<commit_message>
Slack Variable * 10 implemented
</commit_message>
<xml_diff>
--- a/PGY1_Allocations_export.xlsx
+++ b/PGY1_Allocations_export.xlsx
@@ -469,22 +469,22 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
+          <t>BDH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>BDH Emergency (PGY1/2)</t>
+          <t>CMN Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>JHH Medicine - Nephrology &amp; Dialysis (PGY1/2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>JHH General Surgery / Hepatopancreatobiliary and Upper GI Surgery (PGY1/2)</t>
+          <t>MH Emergency (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -545,7 +545,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>50.00</t>
+          <t>100.00</t>
         </is>
       </c>
     </row>
@@ -569,7 +569,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>11.80</t>
+          <t>3.00</t>
         </is>
       </c>
     </row>
@@ -581,7 +581,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>21.50</t>
+          <t>5.00</t>
         </is>
       </c>
     </row>
@@ -593,7 +593,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1.50</t>
+          <t>1.00</t>
         </is>
       </c>
     </row>
@@ -605,7 +605,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>8.95</t>
+          <t>1.58</t>
         </is>
       </c>
     </row>
@@ -737,11 +737,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
+          <t>BDH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C8">
-        <v>38</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -752,11 +752,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>BDH Emergency (PGY1/2)</t>
+          <t>CMN Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
@@ -767,11 +767,11 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>JHH Medicine - Nephrology &amp; Dialysis (PGY1/2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C10">
-        <v>33</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11">
@@ -782,11 +782,11 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>JHH General Surgery / Hepatopancreatobiliary and Upper GI Surgery (PGY1/2)</t>
+          <t>MH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C11">
-        <v>25</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -842,7 +842,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -874,7 +874,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>20.6</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -884,17 +884,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>FALSE</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>TRUE</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
     </row>
@@ -1710,12 +1710,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>BDH Sub-Acute General Medicine (Team 5) (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>BDH Emergency (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>BDH Surgery (PGY1/2)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1737,12 +1737,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>BDH Sub-Acute General Medicine (Team 5) (PGY1/2)</t>
+          <t>BDH Surgery (PGY1/2)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>CMN Emergency (PGY1/2)</t>
+          <t>BDH Surgery (PGY1/2)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1764,7 +1764,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>BDH Surgery (PGY1/2)</t>
+          <t>CMN Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1845,7 +1845,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>CMN Emergency (PGY1/2)</t>
+          <t>CMN General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1953,7 +1953,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>CMN General Medicine (PGY1/2)</t>
+          <t>CMN Medicine - Gastroenterology with Drug &amp; Alcohol (PGY1/2)</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1980,7 +1980,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>CMN Medicine - Gastroenterology with Drug &amp; Alcohol (PGY1/2)</t>
+          <t>CMN Medicine - Haematology (01) (PGY1/2)</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -2007,7 +2007,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>CMN Medicine - Haematology (01) (PGY1/2)</t>
+          <t>CMN Medicine - Medical Oncology (01) (PGY1/2)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -2034,7 +2034,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>CMN Medicine - Medical Oncology (01) (PGY1/2)</t>
+          <t>CMN Palliative Care (PGY1/2)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -2061,7 +2061,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>CMN Palliative Care (PGY1/2)</t>
+          <t>CMN Surgery (PGY1/2)</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -2115,7 +2115,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>CMN Surgery (PGY1/2)</t>
+          <t>HNE Mental Health &amp; Substance Use Service - Mater Hospital (PGY1/2)</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -2142,7 +2142,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>HNE Mental Health &amp; Substance Use Service - Mater Hospital (PGY1/2)</t>
+          <t>HNE Mental Health Lake Macquarie Ward - Mater hospital (PGY1/2)</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -2169,7 +2169,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>HNE Mental Health Lake Macquarie Ward - Mater hospital (PGY1/2)</t>
+          <t>HNE Mental Health Newcastle Inpatient Unit - Mater Hospital (PGY1/2)</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -2196,7 +2196,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>HNE Mental Health Newcastle Inpatient Unit - Mater Hospital (PGY1/2)</t>
+          <t>HNE Mental Health Older People's Service - Mater Hospital (PGY1/2)</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -2223,7 +2223,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>HNE Mental Health Older People's Service - Mater Hospital (PGY1/2)</t>
+          <t>JHH Acute General Surgery Unit (PGY1/2)</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -2277,7 +2277,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>JHH Acute General Surgery Unit (PGY1/2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -2476,7 +2476,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>JHH Emergency (PGY1/2)</t>
+          <t>JHH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -2493,7 +2493,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>JHH Emergency (PGY1/2)</t>
+          <t>JHH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -2584,12 +2584,12 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>JHH General Medicine (PGY1/2)</t>
+          <t>JHH General Surgery / Colorectal (PGY1/2)</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>JHH General Surgery / Trauma (PGY1/2)</t>
+          <t>JHH General Surgery / Hepatopancreatobiliary and Upper GI Surgery (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>JHH General Medicine (PGY1/2)</t>
+          <t>JHH General Surgery / Colorectal (PGY1/2)</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -2611,12 +2611,12 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>JHH General Surgery / Colorectal (PGY1/2)</t>
+          <t>JHH General Surgery / Trauma (PGY1/2)</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>JHH Medicine - Cardiology (PGY1/2)</t>
+          <t>JHH General Surgery / Trauma (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2628,7 +2628,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>JHH General Surgery / Colorectal (PGY1/2)</t>
+          <t>JHH General Surgery / Trauma (PGY1/2)</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -2638,7 +2638,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>JHH General Surgery / Trauma (PGY1/2)</t>
+          <t>JHH Medicine - Cardiology (PGY1/2)</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -2655,7 +2655,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>JHH General Surgery / Trauma (PGY1/2)</t>
+          <t>JHH General Surgery / Upper GI (PGY1/2)</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -2665,12 +2665,12 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
+          <t>JHH Medicine - Dermatology (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
           <t>JHH Medicine - Cardiology (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>JHH Medicine - Gastroenterology (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2682,7 +2682,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>JHH General Surgery / Upper GI (PGY1/2)</t>
+          <t>JHH Medicine - Cardiology (PGY1/2)</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -2692,7 +2692,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>JHH Medicine - Dermatology (PGY1/2)</t>
+          <t>JHH Medicine - Gastroenterology (PGY1/2)</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -2709,7 +2709,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>JHH Medicine - Cardiology (PGY1/2)</t>
+          <t>JHH Medicine - Dermatology (PGY1/2)</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2719,12 +2719,12 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
+          <t>JHH Medicine - MACU (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
           <t>JHH Medicine - Gastroenterology (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>JHH Medicine - Infectious Disease (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2736,7 +2736,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>JHH Medicine - Dermatology (PGY1/2)</t>
+          <t>JHH Medicine - Gastroenterology (PGY1/2)</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2746,12 +2746,12 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>JHH Medicine - MACU (PGY1/2)</t>
+          <t>JHH Medicine - Nephrology &amp; Dialysis (PGY1/2)</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>JHH Medicine - Neurology (PGY1/2)</t>
+          <t>JHH Medicine - Infectious Disease (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2763,7 +2763,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>JHH Medicine - Gastroenterology (PGY1/2)</t>
+          <t>JHH Medicine - MACU (PGY1/2)</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -2778,7 +2778,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>JHH Medicine - Rehabilitation (PGY1/2)</t>
+          <t>JHH Medicine - Neurology (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2790,7 +2790,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>JHH Medicine - MACU (PGY1/2)</t>
+          <t>JHH Medicine - Nephrology &amp; Dialysis (PGY1/2)</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2817,7 +2817,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>JHH Medicine - Nephrology &amp; Dialysis (PGY1/2)</t>
+          <t>JHH Medicine - Neurology (PGY1/2)</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2832,7 +2832,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>JHH Medicine - Respiratory (PGY1/2)</t>
+          <t>JHH Medicine - Rehabilitation (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2844,7 +2844,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>JHH Medicine - Neurology (PGY1/2)</t>
+          <t>JHH Medicine - Rehabilitation (PGY1/2)</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2859,7 +2859,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
+          <t>JHH Medicine - Respiratory (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2886,7 +2886,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>JHH Surgery - Cardiothoracic Surgery (PGY1/2)</t>
+          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2898,7 +2898,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>JHH Medicine - Rehabilitation (PGY1/2)</t>
+          <t>JHH Medicine - Respiratory (PGY1/2)</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2913,7 +2913,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>JHH Surgery - Neurosurgery (PGY1/2)</t>
+          <t>JHH Surgery - Cardiothoracic Surgery (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2952,7 +2952,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>JHH Medicine - Respiratory (PGY1/2)</t>
+          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2967,7 +2967,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
+          <t>JHH Surgery - Neurosurgery (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -3102,7 +3102,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>JHH Surgery - Orthopaedics (Team 6) (PGY1/2)</t>
+          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -3129,7 +3129,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>JHH Surgery - Urology (PGY1/2)</t>
+          <t>JHH Surgery - Orthopaedics (Team 6) (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -3183,7 +3183,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>JHH Surgery - Vascular (PGY1/2)</t>
+          <t>JHH Surgery - Urology (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -3237,7 +3237,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>MH  Medicine - Cardiology (PGY1/2)</t>
+          <t>JHH Surgery - Vascular (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -3264,7 +3264,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>MH Emergency (PGY1/2)</t>
+          <t>MH  Medicine - Cardiology (PGY1/2)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Massive break through with the specialty status of terms. Massive. Functioning now.
</commit_message>
<xml_diff>
--- a/PGY1_Allocations_export.xlsx
+++ b/PGY1_Allocations_export.xlsx
@@ -442,7 +442,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>CMN Medicine - Cardiology (PGY1/2)</t>
+          <t>JHH Surgery - Vascular (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -568,7 +568,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>CMN Medicine - Medical Oncology (01) (PGY1/2)</t>
+          <t>BDH Surgery (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -694,7 +694,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>CMN Relief (PGY1/2)</t>
+          <t>BDH Acute General Medicine &amp; Cardiology (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -731,12 +731,12 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>BDH Acute General Medicine &amp; Rehabilitation (PGY1/2)</t>
+          <t>MH KK Rehabilitation (PGY 1/2)</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>MH  Medicine - Cardiology (PGY1/2)</t>
+          <t>JHH Surgery - Neurosurgery (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -778,7 +778,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>JHH Surgery - Neurosurgery (PGY1/2)</t>
+          <t>CMN Medicine - Haematology (01) (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -815,7 +815,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>JHH Surgery - Neurosurgery (PGY1/2)</t>
+          <t>JHH Medicine - Respiratory (PGY1/2)</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -904,7 +904,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>CMN General Medicine (PGY1/2)</t>
+          <t>JHH Medicine - Rehabilitation (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -936,17 +936,17 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
+          <t>JHH General Medicine (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
           <t>CMN Medicine - Medical Oncology (01) (PGY1/2)</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>JHH General Medicine (PGY1/2)</t>
-        </is>
-      </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>JHH Medicine - Rehabilitation (PGY1/2)</t>
+          <t>MH General Surgery (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -988,7 +988,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>JHH Emergency (PGY1/2)</t>
+          <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -1020,17 +1020,17 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
+          <t>MH Emergency (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>JHH Acute General Surgery Unit (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
           <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>JHH Acute General Surgery Unit (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>MH Emergency (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -1062,7 +1062,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>BDH Surgery (PGY1/2)</t>
+          <t>CMN Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1072,7 +1072,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>JHH Surgery - Urology (PGY1/2)</t>
+          <t>JHH Acute General Surgery Unit (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -1146,17 +1146,17 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>MH General Surgery (PGY1/2)</t>
+          <t>MBH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>MBH Emergency (PGY1/2)</t>
+          <t>HNE Mental Health Newcastle Inpatient Unit - Mater Hospital (PGY1/2)</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>HNE Mental Health Newcastle Inpatient Unit - Mater Hospital (PGY1/2)</t>
+          <t>HNE Mental Health Lake Macquarie Ward - Mater hospital (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -1277,12 +1277,12 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>BDH Sub-Acute General Medicine (Team 5) (PGY1/2)</t>
+          <t>CMN Palliative Care (PGY1/2)</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>JHH General Medicine (PGY1/2)</t>
+          <t>JHH Surgery - Urology (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -1398,7 +1398,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>JHH Medicine Relief (PGY1/2)</t>
+          <t>MH General Surgery (PGY1/2)</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -1408,7 +1408,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>HNE Mental Health Lake Macquarie Ward - Mater hospital (PGY1/2)</t>
+          <t>JHH Medicine - Gastroenterology (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -1445,12 +1445,12 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>JHH Medicine Relief (PGY1/2)</t>
+          <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -1492,7 +1492,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>MH Emergency (PGY1/2)</t>
+          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -1576,7 +1576,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>BDH Acute General Medicine (PGY1/2)</t>
+          <t>CMN Medicine - Cardiology (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>CMN Palliative Care (PGY1/2)</t>
+          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -1650,12 +1650,12 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
+          <t>CMN Emergency (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
           <t>JHH Medicine Relief (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>MH KK Rehabilitation (PGY 1/2)</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -1744,7 +1744,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>JHH Surgery - Vascular (PGY1/2)</t>
+          <t>MH  Medicine - Cardiology (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -1786,7 +1786,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>JHH Medicine - Respiratory (PGY1/2)</t>
+          <t>CMN Relief (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -1823,12 +1823,12 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>CMN Emergency (PGY1/2)</t>
+          <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>CMN General Medicine (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2028,17 +2028,17 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>CMN Medicine - Haematology (01) (PGY1/2)</t>
+          <t>BDH Surgery (PGY1/2)</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>BDH Acute General Medicine (PGY1/2)</t>
+          <t>CMN Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>MH General Medicine (PGY1/2)</t>
+          <t>CMN Surgery (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2122,7 +2122,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>CMN Surgery (PGY1/2)</t>
+          <t>MH Emergency (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2159,12 +2159,12 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>MH General Medicine (PGY1/2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>JHH Emergency (PGY1/2)</t>
+          <t>JHH General Surgery / Hepatopancreatobiliary and Upper GI Surgery (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2233,14 +2233,14 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
+          <t>MH General Medicine (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
           <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>MH General Medicine (PGY1/2)</t>
-        </is>
-      </c>
       <c r="G45" t="inlineStr">
         <is>
           <t>JHH Emergency (PGY1/2)</t>
@@ -2248,7 +2248,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>JHH Medicine - Cardiology (PGY1/2)</t>
+          <t>MH Emergency (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2280,17 +2280,17 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
+          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>CMN Medicine - Gastroenterology with Drug &amp; Alcohol (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
           <t>MH Emergency (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>CMN Medicine - Gastroenterology with Drug &amp; Alcohol (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>CMN Emergency (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2332,7 +2332,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
+          <t>BDH Acute General Medicine (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2364,17 +2364,17 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
+          <t>CMN Relief (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
           <t>BDH Acute General Medicine (PGY1/2)</t>
         </is>
       </c>
-      <c r="G48" t="inlineStr">
+      <c r="H48" t="inlineStr">
         <is>
           <t>JHH Emergency (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>BDH Surgery (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2453,7 +2453,7 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>BDH After Hours Internal Relief (PGY1/2)</t>
+          <t>JHH General Surgery / Upper GI (PGY1/2)</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -2495,12 +2495,12 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
+          <t>MBH Emergency (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
           <t>CMN Relief (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>BDH Acute General Medicine &amp; Cardiology (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2579,12 +2579,12 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>MH General Surgery (PGY1/2)</t>
+          <t>TRRH Surgery C (PGY1/2)</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>JHH Acute General Surgery Unit (PGY1/2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2616,12 +2616,12 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
+          <t>CMN Medicine - Medical Oncology (01) (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
           <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>CMN Medicine - Medical Oncology (01) (PGY1/2)</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
@@ -2658,7 +2658,7 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>MBH Emergency (PGY1/2)</t>
+          <t>BDH Acute General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
@@ -2668,7 +2668,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>JHH Emergency (PGY1/2)</t>
+          <t>BDH After Hours Internal Relief (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2710,7 +2710,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>HNE Mental Health Older People's Service - Mater Hospital (PGY1/2)</t>
+          <t>JHH Medicine - Cardiology (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2794,7 +2794,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>CMN General Medicine (PGY1/2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2831,7 +2831,7 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>TRRH Surgery C (PGY1/2)</t>
+          <t>CMN General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
@@ -2873,12 +2873,12 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
+          <t>JHH Surgery Relief (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
           <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="H60" t="inlineStr">
-        <is>
-          <t>JHH Surgery Relief (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2915,12 +2915,12 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>BDH Surgery (PGY1/2)</t>
+          <t>BDH Sub-Acute General Medicine (Team 5) (PGY1/2)</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>JHH Emergency (PGY1/2)</t>
+          <t>CMN Medicine - Medical Oncology (01) (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2999,7 +2999,7 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
+          <t>CMN Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
@@ -3120,17 +3120,17 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
+          <t>CMN Medicine - Haematology (01) (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
           <t>JHH General Medicine (PGY1/2)</t>
         </is>
       </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>CMN Medicine - Haematology (01) (PGY1/2)</t>
-        </is>
-      </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
+          <t>HNE Mental Health Older People's Service - Mater Hospital (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -3204,17 +3204,17 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>CMN General Medicine (PGY1/2)</t>
+          <t>CMN Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>JHH Medicine - Respiratory (PGY1/2)</t>
+          <t>BDH Surgery (PGY1/2)</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>JHH Medicine - Gastroenterology (PGY1/2)</t>
+          <t>JHH Acute General Surgery Unit (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -3335,12 +3335,12 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>JHH General Surgery / Upper GI (PGY1/2)</t>
+          <t>BDH Acute General Medicine &amp; Rehabilitation (PGY1/2)</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>JHH General Surgery / Hepatopancreatobiliary and Upper GI Surgery (PGY1/2)</t>
+          <t>CMN General Medicine (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -3377,12 +3377,12 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
+          <t>CMN Medicine - Haematology (01) (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
           <t>HNE Mental Health Newcastle Inpatient Unit - Mater Hospital (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="H72" t="inlineStr">
-        <is>
-          <t>CMN Medicine - Haematology (01) (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -3414,17 +3414,17 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>CMN Emergency (PGY1/2)</t>
+          <t>MH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>MH General Medicine (PGY1/2)</t>
+          <t>JHH Surgery - Neurosurgery (PGY1/2)</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>JHH Acute General Surgery Unit (PGY1/2)</t>
+          <t>JHH Medicine - Respiratory (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -3461,12 +3461,12 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>JHH General Medicine (PGY1/2)</t>
+          <t>MH General Surgery (PGY1/2)</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>MH General Surgery (PGY1/2)</t>
+          <t>JHH Medicine - Rehabilitation (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -3503,7 +3503,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>98.63</t>
         </is>
       </c>
     </row>
@@ -3515,7 +3515,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>94.52</t>
+          <t>95.89</t>
         </is>
       </c>
     </row>
@@ -3527,7 +3527,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>76.71</t>
+          <t>71.23</t>
         </is>
       </c>
     </row>
@@ -3539,7 +3539,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>98.63</t>
         </is>
       </c>
     </row>
@@ -3551,7 +3551,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>17.43</t>
+          <t>17.81</t>
         </is>
       </c>
     </row>
@@ -3563,7 +3563,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>43.85</t>
+          <t>45.22</t>
         </is>
       </c>
     </row>
@@ -3575,7 +3575,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1.70</t>
+          <t>2.04</t>
         </is>
       </c>
     </row>
@@ -3587,7 +3587,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>18.97</t>
+          <t>19.53</t>
         </is>
       </c>
     </row>
@@ -3689,11 +3689,11 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CMN Medicine - Cardiology (PGY1/2)</t>
+          <t>JHH Surgery - Vascular (PGY1/2)</t>
         </is>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7">
@@ -3914,11 +3914,11 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>CMN Medicine - Medical Oncology (01) (PGY1/2)</t>
+          <t>BDH Surgery (PGY1/2)</t>
         </is>
       </c>
       <c r="C21">
-        <v>5</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22">
@@ -4139,11 +4139,11 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>CMN Relief (PGY1/2)</t>
+          <t>BDH Acute General Medicine &amp; Cardiology (PGY1/2)</t>
         </is>
       </c>
       <c r="C36">
-        <v>51</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37">
@@ -4199,11 +4199,11 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>BDH Acute General Medicine &amp; Rehabilitation (PGY1/2)</t>
+          <t>MH KK Rehabilitation (PGY 1/2)</t>
         </is>
       </c>
       <c r="C40">
-        <v>35</v>
+        <v>51</v>
       </c>
     </row>
     <row r="41">
@@ -4214,11 +4214,11 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>MH  Medicine - Cardiology (PGY1/2)</t>
+          <t>JHH Surgery - Neurosurgery (PGY1/2)</t>
         </is>
       </c>
       <c r="C41">
-        <v>50</v>
+        <v>19</v>
       </c>
     </row>
     <row r="42">
@@ -4289,11 +4289,11 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>JHH Surgery - Neurosurgery (PGY1/2)</t>
+          <t>CMN Medicine - Haematology (01) (PGY1/2)</t>
         </is>
       </c>
       <c r="C46">
-        <v>39</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47">
@@ -4349,11 +4349,11 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>JHH Surgery - Neurosurgery (PGY1/2)</t>
+          <t>JHH Medicine - Respiratory (PGY1/2)</t>
         </is>
       </c>
       <c r="C50">
-        <v>24</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51">
@@ -4514,11 +4514,11 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>CMN General Medicine (PGY1/2)</t>
+          <t>JHH Medicine - Rehabilitation (PGY1/2)</t>
         </is>
       </c>
       <c r="C61">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="62">
@@ -4559,11 +4559,11 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>CMN Medicine - Medical Oncology (01) (PGY1/2)</t>
+          <t>JHH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="C64">
-        <v>5</v>
+        <v>41</v>
       </c>
     </row>
     <row r="65">
@@ -4574,11 +4574,11 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>JHH General Medicine (PGY1/2)</t>
+          <t>CMN Medicine - Medical Oncology (01) (PGY1/2)</t>
         </is>
       </c>
       <c r="C65">
-        <v>41</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66">
@@ -4589,11 +4589,11 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>JHH Medicine - Rehabilitation (PGY1/2)</t>
+          <t>MH General Surgery (PGY1/2)</t>
         </is>
       </c>
       <c r="C66">
-        <v>29</v>
+        <v>52</v>
       </c>
     </row>
     <row r="67">
@@ -4664,11 +4664,11 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>JHH Emergency (PGY1/2)</t>
+          <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C71">
-        <v>1</v>
+        <v>55</v>
       </c>
     </row>
     <row r="72">
@@ -4709,11 +4709,11 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
+          <t>MH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C74">
-        <v>47</v>
+        <v>26</v>
       </c>
     </row>
     <row r="75">
@@ -4739,11 +4739,11 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>MH Emergency (PGY1/2)</t>
+          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
         </is>
       </c>
       <c r="C76">
-        <v>26</v>
+        <v>47</v>
       </c>
     </row>
     <row r="77">
@@ -4784,11 +4784,11 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>BDH Surgery (PGY1/2)</t>
+          <t>CMN Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C79">
-        <v>44</v>
+        <v>54</v>
       </c>
     </row>
     <row r="80">
@@ -4814,11 +4814,11 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>JHH Surgery - Urology (PGY1/2)</t>
+          <t>JHH Acute General Surgery Unit (PGY1/2)</t>
         </is>
       </c>
       <c r="C81">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="82">
@@ -4934,11 +4934,11 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>MH General Surgery (PGY1/2)</t>
+          <t>MBH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C89">
-        <v>50</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90">
@@ -4949,11 +4949,11 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>MBH Emergency (PGY1/2)</t>
+          <t>HNE Mental Health Newcastle Inpatient Unit - Mater Hospital (PGY1/2)</t>
         </is>
       </c>
       <c r="C90">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="91">
@@ -4964,11 +4964,11 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>HNE Mental Health Newcastle Inpatient Unit - Mater Hospital (PGY1/2)</t>
+          <t>HNE Mental Health Lake Macquarie Ward - Mater hospital (PGY1/2)</t>
         </is>
       </c>
       <c r="C91">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="92">
@@ -5174,11 +5174,11 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>BDH Sub-Acute General Medicine (Team 5) (PGY1/2)</t>
+          <t>CMN Palliative Care (PGY1/2)</t>
         </is>
       </c>
       <c r="C105">
-        <v>31</v>
+        <v>5</v>
       </c>
     </row>
     <row r="106">
@@ -5189,11 +5189,11 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>JHH General Medicine (PGY1/2)</t>
+          <t>JHH Surgery - Urology (PGY1/2)</t>
         </is>
       </c>
       <c r="C106">
-        <v>29</v>
+        <v>41</v>
       </c>
     </row>
     <row r="107">
@@ -5384,11 +5384,11 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>JHH Medicine Relief (PGY1/2)</t>
+          <t>MH General Surgery (PGY1/2)</t>
         </is>
       </c>
       <c r="C119">
-        <v>53</v>
+        <v>42</v>
       </c>
     </row>
     <row r="120">
@@ -5414,11 +5414,11 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>HNE Mental Health Lake Macquarie Ward - Mater hospital (PGY1/2)</t>
+          <t>JHH Medicine - Gastroenterology (PGY1/2)</t>
         </is>
       </c>
       <c r="C121">
-        <v>5</v>
+        <v>28</v>
       </c>
     </row>
     <row r="122">
@@ -5474,11 +5474,11 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>JHH Medicine Relief (PGY1/2)</t>
+          <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C125">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="126">
@@ -5489,11 +5489,11 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C126">
-        <v>59</v>
+        <v>4</v>
       </c>
     </row>
     <row r="127">
@@ -5564,11 +5564,11 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>MH Emergency (PGY1/2)</t>
+          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
         </is>
       </c>
       <c r="C131">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="132">
@@ -5714,11 +5714,11 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>BDH Acute General Medicine (PGY1/2)</t>
+          <t>CMN Medicine - Cardiology (PGY1/2)</t>
         </is>
       </c>
       <c r="C141">
-        <v>46</v>
+        <v>4</v>
       </c>
     </row>
     <row r="142">
@@ -5774,11 +5774,11 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>CMN Palliative Care (PGY1/2)</t>
+          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
         </is>
       </c>
       <c r="C145">
-        <v>5</v>
+        <v>43</v>
       </c>
     </row>
     <row r="146">
@@ -5834,11 +5834,11 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>JHH Medicine Relief (PGY1/2)</t>
+          <t>CMN Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C149">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="150">
@@ -5849,11 +5849,11 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>MH KK Rehabilitation (PGY 1/2)</t>
+          <t>JHH Medicine Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C150">
-        <v>53</v>
+        <v>38</v>
       </c>
     </row>
     <row r="151">
@@ -6014,11 +6014,11 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>JHH Surgery - Vascular (PGY1/2)</t>
+          <t>MH  Medicine - Cardiology (PGY1/2)</t>
         </is>
       </c>
       <c r="C161">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="162">
@@ -6089,11 +6089,11 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>JHH Medicine - Respiratory (PGY1/2)</t>
+          <t>CMN Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C166">
-        <v>1</v>
+        <v>56</v>
       </c>
     </row>
     <row r="167">
@@ -6149,11 +6149,11 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>CMN Emergency (PGY1/2)</t>
+          <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C170">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="171">
@@ -6164,11 +6164,11 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>CMN General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="C171">
-        <v>54</v>
+        <v>16</v>
       </c>
     </row>
     <row r="172">
@@ -6509,11 +6509,11 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>CMN Medicine - Haematology (01) (PGY1/2)</t>
+          <t>BDH Surgery (PGY1/2)</t>
         </is>
       </c>
       <c r="C194">
-        <v>1</v>
+        <v>41</v>
       </c>
     </row>
     <row r="195">
@@ -6524,11 +6524,11 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>BDH Acute General Medicine (PGY1/2)</t>
+          <t>CMN Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C195">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="196">
@@ -6539,11 +6539,11 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>MH General Medicine (PGY1/2)</t>
+          <t>CMN Surgery (PGY1/2)</t>
         </is>
       </c>
       <c r="C196">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="197">
@@ -6689,11 +6689,11 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>CMN Surgery (PGY1/2)</t>
+          <t>MH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C206">
-        <v>41</v>
+        <v>49</v>
       </c>
     </row>
     <row r="207">
@@ -6749,11 +6749,11 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>MH General Medicine (PGY1/2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C210">
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="211">
@@ -6764,11 +6764,11 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>JHH Emergency (PGY1/2)</t>
+          <t>JHH General Surgery / Hepatopancreatobiliary and Upper GI Surgery (PGY1/2)</t>
         </is>
       </c>
       <c r="C211">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="212">
@@ -6869,11 +6869,11 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>MH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="C218">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="219">
@@ -6884,11 +6884,11 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>MH General Medicine (PGY1/2)</t>
+          <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C219">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="220">
@@ -6914,11 +6914,11 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>JHH Medicine - Cardiology (PGY1/2)</t>
+          <t>MH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C221">
-        <v>3</v>
+        <v>47</v>
       </c>
     </row>
     <row r="222">
@@ -6959,11 +6959,11 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>MH Emergency (PGY1/2)</t>
+          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
         </is>
       </c>
       <c r="C224">
-        <v>58</v>
+        <v>2</v>
       </c>
     </row>
     <row r="225">
@@ -6989,11 +6989,11 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>CMN Emergency (PGY1/2)</t>
+          <t>MH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C226">
-        <v>18</v>
+        <v>58</v>
       </c>
     </row>
     <row r="227">
@@ -7064,11 +7064,11 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
+          <t>BDH Acute General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="C231">
-        <v>12</v>
+        <v>38</v>
       </c>
     </row>
     <row r="232">
@@ -7109,11 +7109,11 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>BDH Acute General Medicine (PGY1/2)</t>
+          <t>CMN Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C234">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="235">
@@ -7124,11 +7124,11 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>JHH Emergency (PGY1/2)</t>
+          <t>BDH Acute General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="C235">
-        <v>2</v>
+        <v>44</v>
       </c>
     </row>
     <row r="236">
@@ -7139,11 +7139,11 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>BDH Surgery (PGY1/2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C236">
-        <v>46</v>
+        <v>2</v>
       </c>
     </row>
     <row r="237">
@@ -7274,11 +7274,11 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>BDH After Hours Internal Relief (PGY1/2)</t>
+          <t>JHH General Surgery / Upper GI (PGY1/2)</t>
         </is>
       </c>
       <c r="C245">
-        <v>41</v>
+        <v>4</v>
       </c>
     </row>
     <row r="246">
@@ -7349,11 +7349,11 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>CMN Relief (PGY1/2)</t>
+          <t>MBH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C250">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="251">
@@ -7364,11 +7364,11 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>BDH Acute General Medicine &amp; Cardiology (PGY1/2)</t>
+          <t>CMN Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C251">
-        <v>4</v>
+        <v>50</v>
       </c>
     </row>
     <row r="252">
@@ -7499,11 +7499,11 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>MH General Surgery (PGY1/2)</t>
+          <t>TRRH Surgery C (PGY1/2)</t>
         </is>
       </c>
       <c r="C260">
-        <v>44</v>
+        <v>52</v>
       </c>
     </row>
     <row r="261">
@@ -7514,11 +7514,11 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>JHH Acute General Surgery Unit (PGY1/2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C261">
-        <v>37</v>
+        <v>5</v>
       </c>
     </row>
     <row r="262">
@@ -7559,11 +7559,11 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
+          <t>CMN Medicine - Medical Oncology (01) (PGY1/2)</t>
         </is>
       </c>
       <c r="C264">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="265">
@@ -7574,11 +7574,11 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>CMN Medicine - Medical Oncology (01) (PGY1/2)</t>
+          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
         </is>
       </c>
       <c r="C265">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="266">
@@ -7634,11 +7634,11 @@
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>MBH Emergency (PGY1/2)</t>
+          <t>BDH Acute General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="C269">
-        <v>3</v>
+        <v>30</v>
       </c>
     </row>
     <row r="270">
@@ -7664,11 +7664,11 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>JHH Emergency (PGY1/2)</t>
+          <t>BDH After Hours Internal Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C271">
-        <v>5</v>
+        <v>56</v>
       </c>
     </row>
     <row r="272">
@@ -7739,11 +7739,11 @@
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>HNE Mental Health Older People's Service - Mater Hospital (PGY1/2)</t>
+          <t>JHH Medicine - Cardiology (PGY1/2)</t>
         </is>
       </c>
       <c r="C276">
-        <v>45</v>
+        <v>2</v>
       </c>
     </row>
     <row r="277">
@@ -7889,11 +7889,11 @@
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>CMN General Medicine (PGY1/2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C286">
-        <v>44</v>
+        <v>1</v>
       </c>
     </row>
     <row r="287">
@@ -7949,11 +7949,11 @@
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>TRRH Surgery C (PGY1/2)</t>
+          <t>CMN General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="C290">
-        <v>47</v>
+        <v>13</v>
       </c>
     </row>
     <row r="291">
@@ -8024,11 +8024,11 @@
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
+          <t>JHH Surgery Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C295">
-        <v>5</v>
+        <v>59</v>
       </c>
     </row>
     <row r="296">
@@ -8039,11 +8039,11 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>JHH Surgery Relief (PGY1/2)</t>
+          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
         </is>
       </c>
       <c r="C296">
-        <v>59</v>
+        <v>5</v>
       </c>
     </row>
     <row r="297">
@@ -8099,11 +8099,11 @@
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>BDH Surgery (PGY1/2)</t>
+          <t>BDH Sub-Acute General Medicine (Team 5) (PGY1/2)</t>
         </is>
       </c>
       <c r="C300">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="301">
@@ -8114,11 +8114,11 @@
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>JHH Emergency (PGY1/2)</t>
+          <t>CMN Medicine - Medical Oncology (01) (PGY1/2)</t>
         </is>
       </c>
       <c r="C301">
-        <v>1</v>
+        <v>44</v>
       </c>
     </row>
     <row r="302">
@@ -8249,11 +8249,11 @@
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
+          <t>CMN Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C310">
-        <v>18</v>
+        <v>49</v>
       </c>
     </row>
     <row r="311">
@@ -8459,11 +8459,11 @@
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>JHH General Medicine (PGY1/2)</t>
+          <t>CMN Medicine - Haematology (01) (PGY1/2)</t>
         </is>
       </c>
       <c r="C324">
-        <v>23</v>
+        <v>2</v>
       </c>
     </row>
     <row r="325">
@@ -8474,11 +8474,11 @@
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>CMN Medicine - Haematology (01) (PGY1/2)</t>
+          <t>JHH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="C325">
-        <v>2</v>
+        <v>23</v>
       </c>
     </row>
     <row r="326">
@@ -8489,11 +8489,11 @@
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
+          <t>HNE Mental Health Older People's Service - Mater Hospital (PGY1/2)</t>
         </is>
       </c>
       <c r="C326">
-        <v>4</v>
+        <v>45</v>
       </c>
     </row>
     <row r="327">
@@ -8609,11 +8609,11 @@
       </c>
       <c r="B334" t="inlineStr">
         <is>
-          <t>CMN General Medicine (PGY1/2)</t>
+          <t>CMN Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C334">
-        <v>21</v>
+        <v>38</v>
       </c>
     </row>
     <row r="335">
@@ -8624,11 +8624,11 @@
       </c>
       <c r="B335" t="inlineStr">
         <is>
-          <t>JHH Medicine - Respiratory (PGY1/2)</t>
+          <t>BDH Surgery (PGY1/2)</t>
         </is>
       </c>
       <c r="C335">
-        <v>3</v>
+        <v>33</v>
       </c>
     </row>
     <row r="336">
@@ -8639,11 +8639,11 @@
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>JHH Medicine - Gastroenterology (PGY1/2)</t>
+          <t>JHH Acute General Surgery Unit (PGY1/2)</t>
         </is>
       </c>
       <c r="C336">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="337">
@@ -8849,11 +8849,11 @@
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>JHH General Surgery / Upper GI (PGY1/2)</t>
+          <t>BDH Acute General Medicine &amp; Rehabilitation (PGY1/2)</t>
         </is>
       </c>
       <c r="C350">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="351">
@@ -8864,11 +8864,11 @@
       </c>
       <c r="B351" t="inlineStr">
         <is>
-          <t>JHH General Surgery / Hepatopancreatobiliary and Upper GI Surgery (PGY1/2)</t>
+          <t>CMN General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="C351">
-        <v>3</v>
+        <v>36</v>
       </c>
     </row>
     <row r="352">
@@ -8924,11 +8924,11 @@
       </c>
       <c r="B355" t="inlineStr">
         <is>
-          <t>HNE Mental Health Newcastle Inpatient Unit - Mater Hospital (PGY1/2)</t>
+          <t>CMN Medicine - Haematology (01) (PGY1/2)</t>
         </is>
       </c>
       <c r="C355">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="356">
@@ -8939,11 +8939,11 @@
       </c>
       <c r="B356" t="inlineStr">
         <is>
-          <t>CMN Medicine - Haematology (01) (PGY1/2)</t>
+          <t>HNE Mental Health Newcastle Inpatient Unit - Mater Hospital (PGY1/2)</t>
         </is>
       </c>
       <c r="C356">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="357">
@@ -8984,11 +8984,11 @@
       </c>
       <c r="B359" t="inlineStr">
         <is>
-          <t>CMN Emergency (PGY1/2)</t>
+          <t>MH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="C359">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="360">
@@ -8999,11 +8999,11 @@
       </c>
       <c r="B360" t="inlineStr">
         <is>
-          <t>MH General Medicine (PGY1/2)</t>
+          <t>JHH Surgery - Neurosurgery (PGY1/2)</t>
         </is>
       </c>
       <c r="C360">
-        <v>43</v>
+        <v>25</v>
       </c>
     </row>
     <row r="361">
@@ -9014,11 +9014,11 @@
       </c>
       <c r="B361" t="inlineStr">
         <is>
-          <t>JHH Acute General Surgery Unit (PGY1/2)</t>
+          <t>JHH Medicine - Respiratory (PGY1/2)</t>
         </is>
       </c>
       <c r="C361">
-        <v>38</v>
+        <v>1</v>
       </c>
     </row>
     <row r="362">
@@ -9074,11 +9074,11 @@
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>JHH General Medicine (PGY1/2)</t>
+          <t>MH General Surgery (PGY1/2)</t>
         </is>
       </c>
       <c r="C365">
-        <v>7</v>
+        <v>47</v>
       </c>
     </row>
     <row r="366">
@@ -9089,11 +9089,11 @@
       </c>
       <c r="B366" t="inlineStr">
         <is>
-          <t>MH General Surgery (PGY1/2)</t>
+          <t>JHH Medicine - Rehabilitation (PGY1/2)</t>
         </is>
       </c>
       <c r="C366">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -9149,17 +9149,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>14.2</t>
+          <t>20.6</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -9226,11 +9226,6 @@
           <t>TRUE</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
       <c r="F4" t="inlineStr">
         <is>
           <t>TRUE</t>
@@ -9245,7 +9240,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>21.2</t>
+          <t>26.8</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -9255,7 +9250,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -9314,15 +9309,10 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
         <is>
           <t>TRUE</t>
         </is>
@@ -9341,7 +9331,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>18.2</t>
+          <t>14.6</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -9373,7 +9363,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>29.6</t>
+          <t>26.6</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -9383,17 +9373,17 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
+          <t>TRUE</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
           <t>FALSE</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -9405,7 +9395,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>33.0</t>
+          <t>25.6</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -9418,14 +9408,9 @@
           <t>TRUE</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>TRUE</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>FALSE</t>
         </is>
       </c>
     </row>
@@ -9437,7 +9422,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>14.6</t>
+          <t>10.8</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -9457,7 +9442,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -9501,7 +9486,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>7.8</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -9510,11 +9495,6 @@
         </is>
       </c>
       <c r="D13" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
         <is>
           <t>TRUE</t>
         </is>
@@ -9533,7 +9513,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>24.2</t>
+          <t>28.8</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -9553,7 +9533,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -9565,7 +9545,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>13.8</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -9610,11 +9590,6 @@
           <t>TRUE</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
       <c r="F16" t="inlineStr">
         <is>
           <t>TRUE</t>
@@ -9629,7 +9604,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>15.8</t>
+          <t>17.2</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -9693,7 +9668,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>22.4</t>
+          <t>13.0</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -9713,7 +9688,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
     </row>
@@ -9789,7 +9764,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>23.6</t>
+          <t>20.8</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -9799,7 +9774,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -9809,7 +9784,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -9834,11 +9809,6 @@
           <t>TRUE</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
       <c r="F23" t="inlineStr">
         <is>
           <t>FALSE</t>
@@ -9866,11 +9836,6 @@
           <t>TRUE</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
       <c r="F24" t="inlineStr">
         <is>
           <t>TRUE</t>
@@ -9885,7 +9850,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>39.8</t>
+          <t>42.2</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -9895,7 +9860,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -9905,7 +9870,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -9917,12 +9882,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>24.8</t>
+          <t>14.6</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -9949,7 +9914,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>11.6</t>
+          <t>10.6</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -9958,11 +9923,6 @@
         </is>
       </c>
       <c r="D27" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
         <is>
           <t>TRUE</t>
         </is>
@@ -10013,7 +9973,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>23.0</t>
+          <t>14.6</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -10022,11 +9982,6 @@
         </is>
       </c>
       <c r="D29" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
         <is>
           <t>TRUE</t>
         </is>
@@ -10045,7 +10000,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>13.6</t>
+          <t>21.2</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -10055,17 +10010,12 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
           <t>TRUE</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -10077,7 +10027,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>20.2</t>
+          <t>16.4</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -10090,14 +10040,9 @@
           <t>TRUE</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
     </row>
@@ -10122,11 +10067,6 @@
           <t>TRUE</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
       <c r="F32" t="inlineStr">
         <is>
           <t>TRUE</t>
@@ -10141,7 +10081,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>31.2</t>
+          <t>29.6</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -10150,11 +10090,6 @@
         </is>
       </c>
       <c r="D33" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
         <is>
           <t>TRUE</t>
         </is>
@@ -10173,17 +10108,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>13.8</t>
+          <t>24.8</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
+          <t>FALSE</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
           <t>TRUE</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>FALSE</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -10205,7 +10140,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>29.8</t>
+          <t>23.8</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -10282,11 +10217,6 @@
           <t>TRUE</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
       <c r="F37" t="inlineStr">
         <is>
           <t>TRUE</t>
@@ -10365,7 +10295,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>20.2</t>
+          <t>24.6</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -10375,7 +10305,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -10385,7 +10315,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -10429,7 +10359,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>13.0</t>
+          <t>14.6</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -10438,11 +10368,6 @@
         </is>
       </c>
       <c r="D42" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
         <is>
           <t>TRUE</t>
         </is>
@@ -10461,7 +10386,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>14.8</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -10471,7 +10396,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -10525,7 +10450,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>22.6</t>
+          <t>31.4</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -10535,7 +10460,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -10557,7 +10482,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>16.8</t>
+          <t>13.6</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -10589,7 +10514,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -10621,7 +10546,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>19.6</t>
+          <t>17.8</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -10685,7 +10610,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>22.0</t>
+          <t>14.6</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -10694,11 +10619,6 @@
         </is>
       </c>
       <c r="D50" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
         <is>
           <t>TRUE</t>
         </is>
@@ -10717,7 +10637,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>12.4</t>
+          <t>20.6</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -10727,7 +10647,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -10781,7 +10701,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>23.0</t>
+          <t>18.2</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -10845,7 +10765,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>12.0</t>
+          <t>27.6</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -10855,7 +10775,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -10877,7 +10797,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>22.4</t>
+          <t>13.8</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -10941,7 +10861,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>29.0</t>
+          <t>20.4</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -10961,7 +10881,7 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -10973,7 +10893,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>24.2</t>
+          <t>17.4</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -10982,11 +10902,6 @@
         </is>
       </c>
       <c r="D59" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr">
         <is>
           <t>TRUE</t>
         </is>
@@ -11037,7 +10952,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>15.6</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -11047,7 +10962,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -11057,7 +10972,7 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -11101,7 +11016,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>16.4</t>
+          <t>22.6</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -11178,11 +11093,6 @@
           <t>TRUE</t>
         </is>
       </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
       <c r="F65" t="inlineStr">
         <is>
           <t>TRUE</t>
@@ -11197,7 +11107,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>14.8</t>
+          <t>23.0</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -11261,7 +11171,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>13.2</t>
+          <t>22.8</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -11271,7 +11181,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -11281,7 +11191,7 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -11306,11 +11216,6 @@
           <t>TRUE</t>
         </is>
       </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
       <c r="F69" t="inlineStr">
         <is>
           <t>TRUE</t>
@@ -11338,11 +11243,6 @@
           <t>TRUE</t>
         </is>
       </c>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
       <c r="F70" t="inlineStr">
         <is>
           <t>TRUE</t>
@@ -11357,7 +11257,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>14.6</t>
+          <t>25.2</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -11367,7 +11267,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -11377,7 +11277,7 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -11421,7 +11321,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>32.0</t>
+          <t>22.4</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -11453,7 +11353,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>13.0</t>
+          <t>18.6</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -11463,7 +11363,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -25314,7 +25214,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>JHH General Medicine (PGY1/2)</t>
+          <t>CMN Emergency (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -25336,7 +25236,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>CMN General Medicine (PGY1/2)</t>
+          <t>JHH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -25385,17 +25285,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>CMN General Medicine (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
           <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
-        </is>
-      </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>JHH Medicine - Rehabilitation (PGY1/2)</t>
+          <t>JHH General Medicine (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -25422,7 +25322,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
+          <t>JHH General Medicine (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -25439,7 +25339,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>MH Emergency (PGY1/2)</t>
+          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -25466,7 +25366,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>MH Emergency (PGY1/2)</t>
+          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -25503,7 +25403,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>MH Emergency (PGY1/2)</t>
+          <t>MH General Medicine (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -25520,7 +25420,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>CMN Relief (PGY1/2)</t>
+          <t>MH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -25542,17 +25442,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>MH General Surgery (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>MH Emergency (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
           <t>MH General Medicine (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>CMN Relief (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>CMN Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -25569,22 +25469,22 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>MH General Surgery (PGY1/2)</t>
+          <t>CMN Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
+          <t>HNE Relief (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>MH General Medicine (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
           <t>CMN Relief (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>HNE Relief (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>BDH After Hours Internal Relief (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -25606,12 +25506,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
+          <t>BDH After Hours Internal Relief (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
           <t>HNE Relief (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>CMN Relief (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -25623,22 +25523,22 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>HNE Relief (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>HNE Relief (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
           <t>CMN Relief (PGY1/2)</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>HNE Relief (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>HNE Relief (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>CMN Relief (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -25763,7 +25663,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>JHH Medicine Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -25790,7 +25690,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>JHH Medicine Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -25834,12 +25734,12 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>JHH Medicine Relief (PGY1/2)</t>
+          <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>JHH Surgery Relief (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -25851,7 +25751,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>JHH Surgery Relief (PGY1/2)</t>
+          <t>JHH Medicine Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">

</xml_diff>